<commit_message>
Full Map is Working
Needs:
- Separate out by EL and IEP status
- Make interactive
- Clean up Figures with labs
- Add text to explain
</commit_message>
<xml_diff>
--- a/data/DataVizfinal_names.xlsx
+++ b/data/DataVizfinal_names.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dfainstein/Desktop/R/Final_proj_edld652/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFE24AD5-A1C4-A74A-9048-3701B0643EEB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F9963B-8C47-E14D-9398-11D5B5C8E39F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29820" yWindow="500" windowWidth="22940" windowHeight="14860" xr2:uid="{F9037C27-2B59-B949-A288-97A2ADAD5016}"/>
+    <workbookView xWindow="2060" yWindow="500" windowWidth="25920" windowHeight="15780" xr2:uid="{F9037C27-2B59-B949-A288-97A2ADAD5016}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="104">
   <si>
     <t>SD</t>
   </si>
@@ -343,6 +343,9 @@
   </si>
   <si>
     <t>all_ridings_bc</t>
+  </si>
+  <si>
+    <t>Code</t>
   </si>
 </sst>
 </file>
@@ -720,8 +723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B06895D0-00CC-0649-A923-5629F967FFA5}">
   <dimension ref="A1:E68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" zoomScale="128" zoomScaleNormal="128" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -743,6 +746,9 @@
       <c r="C1" s="4" t="s">
         <v>61</v>
       </c>
+      <c r="D1" s="4" t="s">
+        <v>103</v>
+      </c>
       <c r="E1" s="4" t="s">
         <v>102</v>
       </c>
@@ -757,6 +763,9 @@
       <c r="C2" s="3" t="s">
         <v>75</v>
       </c>
+      <c r="D2" s="3">
+        <v>59015</v>
+      </c>
       <c r="E2" s="3" t="s">
         <v>1</v>
       </c>
@@ -771,6 +780,9 @@
       <c r="C3" s="3" t="s">
         <v>75</v>
       </c>
+      <c r="D3" s="3">
+        <v>59015</v>
+      </c>
       <c r="E3" s="3" t="s">
         <v>63</v>
       </c>
@@ -785,6 +797,9 @@
       <c r="C4" s="3" t="s">
         <v>75</v>
       </c>
+      <c r="D4" s="3">
+        <v>59015</v>
+      </c>
       <c r="E4" s="3" t="s">
         <v>64</v>
       </c>
@@ -799,6 +814,9 @@
       <c r="C5" s="3" t="s">
         <v>75</v>
       </c>
+      <c r="D5" s="3">
+        <v>59015</v>
+      </c>
       <c r="E5" s="3" t="s">
         <v>65</v>
       </c>
@@ -813,6 +831,9 @@
       <c r="C6" s="3" t="s">
         <v>66</v>
       </c>
+      <c r="D6" s="3">
+        <v>59005</v>
+      </c>
       <c r="E6" s="3" t="s">
         <v>66</v>
       </c>
@@ -827,6 +848,9 @@
       <c r="C7" s="3" t="s">
         <v>75</v>
       </c>
+      <c r="D7" s="3">
+        <v>59015</v>
+      </c>
       <c r="E7" s="3" t="s">
         <v>67</v>
       </c>
@@ -841,6 +865,9 @@
       <c r="C8" s="3" t="s">
         <v>77</v>
       </c>
+      <c r="D8" s="3">
+        <v>59017</v>
+      </c>
       <c r="E8" s="3" t="s">
         <v>68</v>
       </c>
@@ -855,6 +882,9 @@
       <c r="C9" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="D9" s="3">
+        <v>59014</v>
+      </c>
       <c r="E9" s="3" t="s">
         <v>69</v>
       </c>
@@ -869,6 +899,9 @@
       <c r="C10" s="3" t="s">
         <v>77</v>
       </c>
+      <c r="D10" s="3">
+        <v>59017</v>
+      </c>
       <c r="E10" s="3" t="s">
         <v>70</v>
       </c>
@@ -883,6 +916,9 @@
       <c r="C11" s="3" t="s">
         <v>77</v>
       </c>
+      <c r="D11" s="3">
+        <v>59017</v>
+      </c>
       <c r="E11" s="3" t="s">
         <v>71</v>
       </c>
@@ -897,6 +933,9 @@
       <c r="C12" s="3" t="s">
         <v>67</v>
       </c>
+      <c r="D12" s="3">
+        <v>59006</v>
+      </c>
       <c r="E12" s="3" t="s">
         <v>2</v>
       </c>
@@ -911,6 +950,9 @@
       <c r="C13" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="D13" s="3">
+        <v>59001</v>
+      </c>
       <c r="E13" s="3" t="s">
         <v>72</v>
       </c>
@@ -925,6 +967,9 @@
       <c r="C14" s="3" t="s">
         <v>76</v>
       </c>
+      <c r="D14" s="3">
+        <v>59016</v>
+      </c>
       <c r="E14" s="3" t="s">
         <v>73</v>
       </c>
@@ -939,6 +984,9 @@
       <c r="C15" s="3" t="s">
         <v>72</v>
       </c>
+      <c r="D15" s="3">
+        <v>59012</v>
+      </c>
       <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -951,6 +999,9 @@
       <c r="C16" s="3" t="s">
         <v>93</v>
       </c>
+      <c r="D16" s="3">
+        <v>59033</v>
+      </c>
       <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -963,6 +1014,9 @@
       <c r="C17" s="3" t="s">
         <v>90</v>
       </c>
+      <c r="D17" s="3">
+        <v>59030</v>
+      </c>
       <c r="E17" s="3"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -975,6 +1029,9 @@
       <c r="C18" s="3" t="s">
         <v>92</v>
       </c>
+      <c r="D18" s="3">
+        <v>59032</v>
+      </c>
       <c r="E18" s="3" t="s">
         <v>74</v>
       </c>
@@ -989,6 +1046,9 @@
       <c r="C19" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="D19" s="3">
+        <v>59011</v>
+      </c>
       <c r="E19" s="3" t="s">
         <v>75</v>
       </c>
@@ -1003,6 +1063,9 @@
       <c r="C20" s="3" t="s">
         <v>85</v>
       </c>
+      <c r="D20" s="3">
+        <v>59025</v>
+      </c>
       <c r="E20" s="3" t="s">
         <v>76</v>
       </c>
@@ -1017,6 +1080,9 @@
       <c r="C21" s="3" t="s">
         <v>96</v>
       </c>
+      <c r="D21" s="3">
+        <v>59036</v>
+      </c>
       <c r="E21" s="3"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -1029,6 +1095,9 @@
       <c r="C22" s="3" t="s">
         <v>95</v>
       </c>
+      <c r="D22" s="3">
+        <v>59035</v>
+      </c>
       <c r="E22" s="3"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -1041,6 +1110,9 @@
       <c r="C23" s="3" t="s">
         <v>98</v>
       </c>
+      <c r="D23" s="3">
+        <v>59038</v>
+      </c>
       <c r="E23" s="3"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -1053,6 +1125,9 @@
       <c r="C24" s="3" t="s">
         <v>99</v>
       </c>
+      <c r="D24" s="3">
+        <v>59039</v>
+      </c>
       <c r="E24" s="3"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -1065,6 +1140,9 @@
       <c r="C25" s="3" t="s">
         <v>100</v>
       </c>
+      <c r="D25" s="3">
+        <v>59040</v>
+      </c>
       <c r="E25" s="3"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -1077,6 +1155,9 @@
       <c r="C26" s="3" t="s">
         <v>94</v>
       </c>
+      <c r="D26" s="3">
+        <v>59034</v>
+      </c>
       <c r="E26" s="3" t="s">
         <v>77</v>
       </c>
@@ -1091,6 +1172,9 @@
       <c r="C27" s="3" t="s">
         <v>79</v>
       </c>
+      <c r="D27" s="3">
+        <v>59019</v>
+      </c>
       <c r="E27" s="3" t="s">
         <v>78</v>
       </c>
@@ -1105,6 +1189,9 @@
       <c r="C28" s="3" t="s">
         <v>64</v>
       </c>
+      <c r="D28" s="3">
+        <v>59003</v>
+      </c>
       <c r="E28" s="3" t="s">
         <v>79</v>
       </c>
@@ -1119,6 +1206,9 @@
       <c r="C29" s="3" t="s">
         <v>82</v>
       </c>
+      <c r="D29" s="3">
+        <v>59022</v>
+      </c>
       <c r="E29" s="3" t="s">
         <v>80</v>
       </c>
@@ -1133,6 +1223,9 @@
       <c r="C30" s="3" t="s">
         <v>69</v>
       </c>
+      <c r="D30" s="3">
+        <v>59008</v>
+      </c>
       <c r="E30" s="3" t="s">
         <v>81</v>
       </c>
@@ -1147,6 +1240,9 @@
       <c r="C31" s="3" t="s">
         <v>81</v>
       </c>
+      <c r="D31" s="3">
+        <v>59021</v>
+      </c>
       <c r="E31" s="3" t="s">
         <v>82</v>
       </c>
@@ -1161,6 +1257,9 @@
       <c r="C32" s="3" t="s">
         <v>101</v>
       </c>
+      <c r="D32" s="3">
+        <v>59042</v>
+      </c>
       <c r="E32" s="3" t="s">
         <v>83</v>
       </c>
@@ -1175,6 +1274,9 @@
       <c r="C33" s="3" t="s">
         <v>101</v>
       </c>
+      <c r="D33" s="3">
+        <v>59042</v>
+      </c>
       <c r="E33" s="3" t="s">
         <v>84</v>
       </c>
@@ -1189,6 +1291,9 @@
       <c r="C34" s="3" t="s">
         <v>97</v>
       </c>
+      <c r="D34" s="3">
+        <v>59037</v>
+      </c>
       <c r="E34" s="3" t="s">
         <v>85</v>
       </c>
@@ -1203,6 +1308,9 @@
       <c r="C35" s="3" t="s">
         <v>101</v>
       </c>
+      <c r="D35" s="3">
+        <v>59042</v>
+      </c>
       <c r="E35" s="3" t="s">
         <v>86</v>
       </c>
@@ -1217,6 +1325,9 @@
       <c r="C36" s="3" t="s">
         <v>97</v>
       </c>
+      <c r="D36" s="3">
+        <v>59037</v>
+      </c>
       <c r="E36" s="3" t="s">
         <v>87</v>
       </c>
@@ -1231,6 +1342,9 @@
       <c r="C37" s="3" t="s">
         <v>97</v>
       </c>
+      <c r="D37" s="3">
+        <v>59037</v>
+      </c>
       <c r="E37" s="3" t="s">
         <v>88</v>
       </c>
@@ -1245,6 +1359,9 @@
       <c r="C38" s="3" t="s">
         <v>66</v>
       </c>
+      <c r="D38" s="3">
+        <v>59005</v>
+      </c>
       <c r="E38" s="3" t="s">
         <v>89</v>
       </c>
@@ -1259,6 +1376,9 @@
       <c r="C39" s="3" t="s">
         <v>97</v>
       </c>
+      <c r="D39" s="3">
+        <v>59037</v>
+      </c>
       <c r="E39" s="3" t="s">
         <v>90</v>
       </c>
@@ -1273,6 +1393,9 @@
       <c r="C40" s="3" t="s">
         <v>89</v>
       </c>
+      <c r="D40" s="3">
+        <v>59029</v>
+      </c>
       <c r="E40" s="3" t="s">
         <v>91</v>
       </c>
@@ -1287,6 +1410,9 @@
       <c r="C41" s="3" t="s">
         <v>65</v>
       </c>
+      <c r="D41" s="3">
+        <v>59004</v>
+      </c>
       <c r="E41" s="3" t="s">
         <v>92</v>
       </c>
@@ -1301,6 +1427,9 @@
       <c r="C42" s="3" t="s">
         <v>84</v>
       </c>
+      <c r="D42" s="3">
+        <v>59024</v>
+      </c>
       <c r="E42" s="3" t="s">
         <v>93</v>
       </c>
@@ -1315,6 +1444,9 @@
       <c r="C43" s="3" t="s">
         <v>66</v>
       </c>
+      <c r="D43" s="3">
+        <v>59005</v>
+      </c>
       <c r="E43" s="3" t="s">
         <v>94</v>
       </c>
@@ -1329,6 +1461,9 @@
       <c r="C44" s="3" t="s">
         <v>84</v>
       </c>
+      <c r="D44" s="3">
+        <v>59024</v>
+      </c>
       <c r="E44" s="3" t="s">
         <v>95</v>
       </c>
@@ -1343,6 +1478,9 @@
       <c r="C45" s="3" t="s">
         <v>84</v>
       </c>
+      <c r="D45" s="3">
+        <v>59024</v>
+      </c>
       <c r="E45" s="3" t="s">
         <v>96</v>
       </c>
@@ -1357,6 +1495,9 @@
       <c r="C46" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="D46" s="3">
+        <v>59041</v>
+      </c>
       <c r="E46" s="3" t="s">
         <v>97</v>
       </c>
@@ -1371,6 +1512,9 @@
       <c r="C47" s="3" t="s">
         <v>86</v>
       </c>
+      <c r="D47" s="3">
+        <v>59026</v>
+      </c>
       <c r="E47" s="3" t="s">
         <v>98</v>
       </c>
@@ -1385,6 +1529,9 @@
       <c r="C48" s="3" t="s">
         <v>87</v>
       </c>
+      <c r="D48" s="3">
+        <v>59027</v>
+      </c>
       <c r="E48" s="3" t="s">
         <v>99</v>
       </c>
@@ -1399,6 +1546,9 @@
       <c r="C49" s="3" t="s">
         <v>87</v>
       </c>
+      <c r="D49" s="3">
+        <v>59027</v>
+      </c>
       <c r="E49" s="3" t="s">
         <v>100</v>
       </c>
@@ -1413,6 +1563,9 @@
       <c r="C50" s="3" t="s">
         <v>89</v>
       </c>
+      <c r="D50" s="3">
+        <v>59029</v>
+      </c>
       <c r="E50" s="3" t="s">
         <v>4</v>
       </c>
@@ -1427,6 +1580,9 @@
       <c r="C51" s="3" t="s">
         <v>78</v>
       </c>
+      <c r="D51" s="3">
+        <v>59018</v>
+      </c>
       <c r="E51" s="3" t="s">
         <v>101</v>
       </c>
@@ -1441,6 +1597,9 @@
       <c r="C52" s="3" t="s">
         <v>78</v>
       </c>
+      <c r="D52" s="3">
+        <v>59018</v>
+      </c>
       <c r="E52" s="1">
         <v>39</v>
       </c>
@@ -1455,6 +1614,9 @@
       <c r="C53" s="3" t="s">
         <v>70</v>
       </c>
+      <c r="D53" s="3">
+        <v>59009</v>
+      </c>
       <c r="E53" s="1">
         <v>40</v>
       </c>
@@ -1469,6 +1631,9 @@
       <c r="C54" s="3" t="s">
         <v>97</v>
       </c>
+      <c r="D54" s="3">
+        <v>59037</v>
+      </c>
       <c r="E54" s="1">
         <v>41</v>
       </c>
@@ -1483,6 +1648,9 @@
       <c r="C55" s="3" t="s">
         <v>97</v>
       </c>
+      <c r="D55" s="3">
+        <v>59037</v>
+      </c>
       <c r="E55" s="1">
         <v>42</v>
       </c>
@@ -1497,6 +1665,9 @@
       <c r="C56" s="3" t="s">
         <v>73</v>
       </c>
+      <c r="D56" s="3">
+        <v>59013</v>
+      </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57">
@@ -1508,6 +1679,9 @@
       <c r="C57" s="3" t="s">
         <v>67</v>
       </c>
+      <c r="D57" s="3">
+        <v>59006</v>
+      </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58">
@@ -1519,6 +1693,9 @@
       <c r="C58" s="3" t="s">
         <v>67</v>
       </c>
+      <c r="D58" s="3">
+        <v>59006</v>
+      </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59">
@@ -1530,6 +1707,9 @@
       <c r="C59" s="3" t="s">
         <v>67</v>
       </c>
+      <c r="D59" s="3">
+        <v>59006</v>
+      </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60">
@@ -1541,6 +1721,9 @@
       <c r="C60" s="3" t="s">
         <v>71</v>
       </c>
+      <c r="D60" s="3">
+        <v>59010</v>
+      </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61">
@@ -1552,6 +1735,9 @@
       <c r="C61" s="3" t="s">
         <v>84</v>
       </c>
+      <c r="D61" s="3">
+        <v>59024</v>
+      </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62">
@@ -1563,6 +1749,9 @@
       <c r="C62" s="3" t="s">
         <v>88</v>
       </c>
+      <c r="D62" s="3">
+        <v>59028</v>
+      </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63">
@@ -1574,6 +1763,9 @@
       <c r="C63" s="3" t="s">
         <v>80</v>
       </c>
+      <c r="D63" s="3">
+        <v>59020</v>
+      </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64">
@@ -1585,8 +1777,11 @@
       <c r="C64" s="3" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D64" s="3">
+        <v>59037</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>85</v>
       </c>
@@ -1596,8 +1791,11 @@
       <c r="C65" s="3" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D65" s="3">
+        <v>59037</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>87</v>
       </c>
@@ -1607,8 +1805,11 @@
       <c r="C66" s="3" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D66" s="3">
+        <v>59028</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>91</v>
       </c>
@@ -1618,8 +1819,11 @@
       <c r="C67" s="3" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D67" s="3">
+        <v>59028</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>92</v>
       </c>
@@ -1628,6 +1832,9 @@
       </c>
       <c r="C68" s="3" t="s">
         <v>88</v>
+      </c>
+      <c r="D68" s="3">
+        <v>59028</v>
       </c>
     </row>
   </sheetData>

</xml_diff>